<commit_message>
Updated RTL Description Doc
changed i2si_en to rf_i2si_en
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -218,9 +218,6 @@
     <t>Right Parallel Digital Audio</t>
   </si>
   <si>
-    <t>i2si_en</t>
-  </si>
-  <si>
     <t>rf_bist_start_val</t>
   </si>
   <si>
@@ -416,6 +413,9 @@
   </si>
   <si>
     <t>filter coeffecient</t>
+  </si>
+  <si>
+    <t>rf_i2si_en</t>
   </si>
 </sst>
 </file>
@@ -851,8 +851,8 @@
   </sheetPr>
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +924,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -939,7 +939,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -948,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>30</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>36</v>
@@ -1100,7 +1100,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -1115,7 +1115,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
@@ -1130,7 +1130,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
@@ -1145,7 +1145,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -1160,7 +1160,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -1175,7 +1175,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
@@ -1190,7 +1190,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
@@ -1205,7 +1205,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -1220,7 +1220,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
@@ -1235,7 +1235,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1250,7 +1250,7 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -1259,13 +1259,13 @@
         <v>11</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>5</v>
@@ -1274,12 +1274,12 @@
         <v>8</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>36</v>
@@ -1321,7 +1321,7 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
@@ -1336,7 +1336,7 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1351,7 +1351,7 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1366,7 +1366,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1381,7 +1381,7 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
@@ -1396,7 +1396,7 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
@@ -1411,7 +1411,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>36</v>
@@ -1557,22 +1557,22 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D48" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>8</v>
@@ -1581,37 +1581,37 @@
         <v>16</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D50" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>56</v>
+        <v>124</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D51" s="2">
         <v>1</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1632,7 +1632,7 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>5</v>
@@ -1641,28 +1641,28 @@
         <v>16</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="2">
+        <v>8</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="2">
-        <v>8</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>5</v>
@@ -1671,12 +1671,12 @@
         <v>16</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>36</v>
@@ -1718,7 +1718,7 @@
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>8</v>
@@ -1733,7 +1733,7 @@
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>5</v>
@@ -1748,7 +1748,7 @@
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>8</v>
@@ -1763,7 +1763,7 @@
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>5</v>
@@ -1793,7 +1793,7 @@
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>5</v>
@@ -1808,7 +1808,7 @@
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>5</v>
@@ -1823,7 +1823,7 @@
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>5</v>
@@ -1838,7 +1838,7 @@
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>8</v>
@@ -1853,7 +1853,7 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>5</v>
@@ -1862,13 +1862,13 @@
         <v>16</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>8</v>
@@ -1877,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1924,7 +1924,7 @@
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>5</v>
@@ -1939,7 +1939,7 @@
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>5</v>
@@ -1954,7 +1954,7 @@
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>5</v>
@@ -1969,7 +1969,7 @@
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>8</v>
@@ -1984,7 +1984,7 @@
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>8</v>
@@ -1999,7 +1999,7 @@
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>8</v>
@@ -2014,7 +2014,7 @@
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>8</v>
@@ -2029,7 +2029,7 @@
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>5</v>
@@ -2044,7 +2044,7 @@
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>5</v>
@@ -2053,28 +2053,28 @@
         <v>4</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>5</v>
@@ -2083,7 +2083,7 @@
         <v>16</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Interface Spreadsheet for I2S Input
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary\Documents\GitHub\Chip-Design\proj_asic\docs\"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="133">
   <si>
     <t>Direction</t>
   </si>
@@ -191,31 +191,10 @@
     <t>Ready to Send</t>
   </si>
   <si>
-    <t>i2s input is enabled</t>
-  </si>
-  <si>
     <t>ro_fifo_overrrun</t>
   </si>
   <si>
     <t>Input Audio FIFO Overrun</t>
-  </si>
-  <si>
-    <t>rf_bist_en</t>
-  </si>
-  <si>
-    <t>Built in Self-Test (BIST)</t>
-  </si>
-  <si>
-    <t>i2si_lft</t>
-  </si>
-  <si>
-    <t>Left Parallel Digital Audio</t>
-  </si>
-  <si>
-    <t>i2si_rgt</t>
-  </si>
-  <si>
-    <t>Right Parallel Digital Audio</t>
   </si>
   <si>
     <t>rf_bist_start_val</t>
@@ -417,11 +396,56 @@
   <si>
     <t>rf_i2si_en</t>
   </si>
+  <si>
+    <t>inp_sck</t>
+  </si>
+  <si>
+    <t>inp_ws</t>
+  </si>
+  <si>
+    <t>inp_sd</t>
+  </si>
+  <si>
+    <t>Enable bit for deserializer</t>
+  </si>
+  <si>
+    <t>rf_mux_en</t>
+  </si>
+  <si>
+    <t>Select BIST of deserializer</t>
+  </si>
+  <si>
+    <t>i2si_data</t>
+  </si>
+  <si>
+    <t>Parallel Digital Audio</t>
+  </si>
+  <si>
+    <t>trig_fifo_overrun_clr</t>
+  </si>
+  <si>
+    <t>Signal to reset FIFO Overrun</t>
+  </si>
+  <si>
+    <t>sync_sck</t>
+  </si>
+  <si>
+    <t>Synchronized Serial Clock</t>
+  </si>
+  <si>
+    <t>sck_transition</t>
+  </si>
+  <si>
+    <t>needs to be added</t>
+  </si>
+  <si>
+    <t>Serial Clock Transition</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -536,7 +560,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -561,6 +585,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -849,10 +876,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +951,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -939,7 +966,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -948,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1044,7 +1071,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>30</v>
@@ -1058,7 +1085,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>36</v>
@@ -1100,7 +1127,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -1115,7 +1142,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
@@ -1130,7 +1157,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
@@ -1145,7 +1172,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -1160,7 +1187,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -1175,7 +1202,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
@@ -1190,7 +1217,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
@@ -1205,7 +1232,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -1220,7 +1247,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
@@ -1235,7 +1262,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1250,7 +1277,7 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -1259,13 +1286,13 @@
         <v>11</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="9" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>5</v>
@@ -1274,12 +1301,12 @@
         <v>8</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>36</v>
@@ -1321,7 +1348,7 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
@@ -1336,7 +1363,7 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1351,7 +1378,7 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1366,7 +1393,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1381,7 +1408,7 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
@@ -1396,7 +1423,7 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
@@ -1411,7 +1438,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
@@ -1440,7 +1467,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>36</v>
@@ -1482,7 +1509,7 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>5</v>
@@ -1497,7 +1524,7 @@
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
@@ -1512,7 +1539,7 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>5</v>
@@ -1527,7 +1554,7 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>5</v>
@@ -1536,73 +1563,73 @@
         <v>1</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D47" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="2">
+        <v>8</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="2">
-        <v>16</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="2">
+        <v>32</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="2">
-        <v>16</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D50" s="2">
         <v>1</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>124</v>
+        <v>51</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>5</v>
@@ -1611,129 +1638,131 @@
         <v>1</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D52" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D53" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>67</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D55" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="1">
-        <v>1</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="1">
-        <v>1</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D59" s="1">
         <v>1</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>5</v>
@@ -1742,13 +1771,13 @@
         <v>1</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>8</v>
@@ -1757,13 +1786,13 @@
         <v>1</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>5</v>
@@ -1772,13 +1801,13 @@
         <v>1</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
@@ -1787,88 +1816,88 @@
         <v>1</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D64" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D65" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D66" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D67" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="B68" s="7" t="s">
-        <v>116</v>
+      <c r="B68" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D68" s="1">
-        <v>16</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>117</v>
+        <v>1</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>8</v>
@@ -1877,189 +1906,189 @@
         <v>1</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="1"/>
+      <c r="B70" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="1">
+        <v>16</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="1">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" s="2">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="2">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="2" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D73" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="2" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D75" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D76" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D77" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D78" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D79" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D80" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D81" s="2">
-        <v>4</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>113</v>
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>5</v>
@@ -2067,23 +2096,53 @@
       <c r="D82" s="2">
         <v>1</v>
       </c>
-      <c r="E82" s="6" t="s">
-        <v>115</v>
+      <c r="E82" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="2" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D83" s="2">
+        <v>4</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="2">
         <v>16</v>
       </c>
-      <c r="E83" s="6" t="s">
-        <v>123</v>
+      <c r="E85" s="6" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added I2S Output to chip.v
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="131">
   <si>
     <t>Direction</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>Upper Limit</t>
-  </si>
-  <si>
-    <t>input audio fifo underrun</t>
   </si>
   <si>
     <t>i2c</t>
@@ -307,30 +304,6 @@
     </r>
   </si>
   <si>
-    <t>i2so_sck_out</t>
-  </si>
-  <si>
-    <t>i2so_sck_in</t>
-  </si>
-  <si>
-    <t>i2so_ws_out</t>
-  </si>
-  <si>
-    <t>i2so_ws_in</t>
-  </si>
-  <si>
-    <t>i2so_lft</t>
-  </si>
-  <si>
-    <t>i2so_rgt</t>
-  </si>
-  <si>
-    <t>i2so_rts</t>
-  </si>
-  <si>
-    <t>i2so_rtr</t>
-  </si>
-  <si>
     <t>ro_fifo_underrun</t>
   </si>
   <si>
@@ -370,12 +343,6 @@
     <t>1- performs clipping 0- no cliping</t>
   </si>
   <si>
-    <t>rf_i2so_clk2sck_div</t>
-  </si>
-  <si>
-    <t>half of the clock frequency divided by this #</t>
-  </si>
-  <si>
     <t>rf_i2c_reg_indir_addr</t>
   </si>
   <si>
@@ -436,10 +403,37 @@
     <t>sck_transition</t>
   </si>
   <si>
-    <t>needs to be added</t>
-  </si>
-  <si>
     <t>Serial Clock Transition</t>
+  </si>
+  <si>
+    <t>sync_sck_transition</t>
+  </si>
+  <si>
+    <t>rst_n</t>
+  </si>
+  <si>
+    <t>sck_inp</t>
+  </si>
+  <si>
+    <t>Serial Clock Level to Pulse Converter</t>
+  </si>
+  <si>
+    <t>filt_rts</t>
+  </si>
+  <si>
+    <t>filt_data</t>
+  </si>
+  <si>
+    <t>filt_rtr</t>
+  </si>
+  <si>
+    <t>trig_fifo_underrun</t>
+  </si>
+  <si>
+    <t>Signal to reset FIFO Underrun</t>
+  </si>
+  <si>
+    <t>Output Audio FIFO Underrun</t>
   </si>
 </sst>
 </file>
@@ -492,7 +486,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,12 +508,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,7 +548,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -578,13 +566,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -876,10 +861,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +936,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -966,7 +951,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -975,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1071,7 +1056,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>30</v>
@@ -1085,7 +1070,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>36</v>
@@ -1127,7 +1112,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -1142,7 +1127,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
@@ -1157,7 +1142,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
@@ -1172,7 +1157,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -1187,7 +1172,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -1202,7 +1187,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
@@ -1217,7 +1202,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
@@ -1232,7 +1217,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -1247,7 +1232,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
@@ -1262,7 +1247,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1276,8 +1261,8 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="8" t="s">
-        <v>111</v>
+      <c r="B27" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -1285,14 +1270,14 @@
       <c r="D27" s="2">
         <v>11</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>113</v>
+      <c r="E27" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="9" t="s">
-        <v>112</v>
+      <c r="B28" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>5</v>
@@ -1300,13 +1285,13 @@
       <c r="D28" s="2">
         <v>8</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>114</v>
+      <c r="E28" s="8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>36</v>
@@ -1348,7 +1333,7 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
@@ -1363,7 +1348,7 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1378,7 +1363,7 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1393,7 +1378,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1408,7 +1393,7 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
@@ -1423,7 +1408,7 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
@@ -1438,7 +1423,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
@@ -1467,7 +1452,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>36</v>
@@ -1494,7 +1479,7 @@
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>5</v>
@@ -1509,7 +1494,7 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>5</v>
@@ -1524,7 +1509,7 @@
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
@@ -1539,7 +1524,7 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>5</v>
@@ -1554,7 +1539,7 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>5</v>
@@ -1563,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1614,7 +1599,7 @@
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>5</v>
@@ -1623,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1644,7 +1629,7 @@
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>8</v>
@@ -1653,7 +1638,7 @@
         <v>32</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1674,7 +1659,7 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>5</v>
@@ -1683,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1704,7 +1689,7 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>8</v>
@@ -1713,15 +1698,13 @@
         <v>1</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
-        <v>131</v>
-      </c>
+      <c r="A57" s="9"/>
       <c r="B57" s="2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>8</v>
@@ -1730,12 +1713,12 @@
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>36</v>
@@ -1777,10 +1760,10 @@
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D61" s="1">
         <v>1</v>
@@ -1792,7 +1775,7 @@
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>5</v>
@@ -1801,43 +1784,43 @@
         <v>1</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D63" s="1">
         <v>1</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D64" s="1">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>8</v>
@@ -1846,114 +1829,114 @@
         <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D66" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D67" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D69" s="1">
         <v>1</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="B70" s="7" t="s">
-        <v>109</v>
+      <c r="B70" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D70" s="1">
-        <v>16</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>110</v>
+        <v>1</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="1">
-        <v>1</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="A71" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A72" s="4"/>
       <c r="B72" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>5</v>
@@ -1962,28 +1945,28 @@
         <v>1</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="2" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>5</v>
@@ -1992,58 +1975,58 @@
         <v>16</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D76" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D78" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>8</v>
@@ -2052,97 +2035,82 @@
         <v>16</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D80" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D81" s="2">
         <v>1</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>25</v>
+        <v>4</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D83" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D84" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D85" s="2">
-        <v>16</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Filter Interfaces to chip.v
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="132">
   <si>
     <t>Direction</t>
   </si>
@@ -92,12 +92,6 @@
     <t>digital audio serial data</t>
   </si>
   <si>
-    <t>left parllel digtal audio</t>
-  </si>
-  <si>
-    <t>right parllel digital audio</t>
-  </si>
-  <si>
     <t>will turn into sticky bit</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>in/out</t>
   </si>
   <si>
-    <t>read registers for direction and value</t>
-  </si>
-  <si>
     <t>I2C serial clock</t>
   </si>
   <si>
@@ -284,53 +275,9 @@
     <t>i2so</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>block?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>_gpio</t>
-    </r>
-  </si>
-  <si>
     <t>ro_fifo_underrun</t>
   </si>
   <si>
-    <t>filter_aud_in_lft</t>
-  </si>
-  <si>
-    <t>filter_aud_in_rgt</t>
-  </si>
-  <si>
-    <t>filter_aud_in_rts</t>
-  </si>
-  <si>
-    <t>filter_aud_in_rtr</t>
-  </si>
-  <si>
-    <t>filter_aud_out_lft</t>
-  </si>
-  <si>
-    <t>filter_aud_out_rgt</t>
-  </si>
-  <si>
-    <t>filter_aud_out_rts</t>
-  </si>
-  <si>
-    <t>filter_aud_out_rtr</t>
-  </si>
-  <si>
     <t>rf_filter_shift</t>
   </si>
   <si>
@@ -434,6 +381,45 @@
   </si>
   <si>
     <t>Output Audio FIFO Underrun</t>
+  </si>
+  <si>
+    <t>rstb</t>
+  </si>
+  <si>
+    <t>aud_in</t>
+  </si>
+  <si>
+    <t>Input Parallel Digital Audio</t>
+  </si>
+  <si>
+    <t>aud_in_rtr</t>
+  </si>
+  <si>
+    <t>aud_in_rts</t>
+  </si>
+  <si>
+    <t>ready to send (for input FIFO)</t>
+  </si>
+  <si>
+    <t>ready to receive (for input FIFO)</t>
+  </si>
+  <si>
+    <t>aud_out</t>
+  </si>
+  <si>
+    <t>Output Parallel Digital Audio</t>
+  </si>
+  <si>
+    <t>aud_out_rts</t>
+  </si>
+  <si>
+    <t>ready to send (for output FIFO)</t>
+  </si>
+  <si>
+    <t>aud_out_rtr</t>
+  </si>
+  <si>
+    <t>ready to receive (for output FIFO)</t>
   </si>
 </sst>
 </file>
@@ -486,7 +472,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,6 +501,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -548,7 +540,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -573,6 +565,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -861,10 +856,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +891,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -906,7 +901,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -915,13 +910,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -936,7 +931,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -945,28 +940,28 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -975,13 +970,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -990,13 +985,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -1005,13 +1000,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -1020,13 +1015,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
@@ -1035,13 +1030,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
@@ -1050,39 +1045,39 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="1">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -1091,46 +1086,46 @@
         <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="2">
-        <v>1</v>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
@@ -1142,37 +1137,37 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>7</v>
+      <c r="D19" s="2">
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -1181,129 +1176,129 @@
         <v>32</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="2" t="s">
-        <v>72</v>
+      <c r="B26" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="2">
-        <v>1</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="7" t="s">
-        <v>100</v>
+      <c r="B27" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="2">
-        <v>11</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>102</v>
+        <v>8</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2">
-        <v>8</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>103</v>
-      </c>
+      <c r="A28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
@@ -1312,13 +1307,13 @@
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>5</v>
@@ -1327,28 +1322,28 @@
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="1">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1357,114 +1352,114 @@
         <v>32</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="1">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="1">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D37" s="1">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A39" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>5</v>
@@ -1473,13 +1468,13 @@
         <v>1</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>5</v>
@@ -1488,13 +1483,13 @@
         <v>1</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>5</v>
@@ -1503,13 +1498,13 @@
         <v>1</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
@@ -1518,13 +1513,13 @@
         <v>1</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>5</v>
@@ -1533,73 +1528,73 @@
         <v>1</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="2">
+        <v>8</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="2">
-        <v>32</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="2">
+        <v>32</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="2">
-        <v>8</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>5</v>
@@ -1608,73 +1603,73 @@
         <v>1</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D51" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D52" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>8</v>
@@ -1683,13 +1678,13 @@
         <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
+      <c r="A56" s="9"/>
       <c r="B56" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>8</v>
@@ -1698,39 +1693,39 @@
         <v>1</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="9"/>
-      <c r="B57" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>120</v>
-      </c>
+      <c r="A57" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="1">
+        <v>1</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>5</v>
@@ -1739,13 +1734,13 @@
         <v>1</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>5</v>
@@ -1754,13 +1749,13 @@
         <v>1</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>5</v>
@@ -1769,13 +1764,13 @@
         <v>1</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>19</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>5</v>
@@ -1784,43 +1779,43 @@
         <v>1</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>124</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D63" s="1">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D64" s="1">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>114</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>8</v>
@@ -1829,13 +1824,13 @@
         <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>8</v>
@@ -1844,13 +1839,13 @@
         <v>1</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>8</v>
@@ -1859,69 +1854,69 @@
         <v>1</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D69" s="1">
         <v>1</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="1">
-        <v>1</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="A70" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A71" s="4"/>
       <c r="B71" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="2">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="2" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>5</v>
@@ -1930,73 +1925,73 @@
         <v>1</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="2" t="s">
-        <v>38</v>
+        <v>120</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D73" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="2" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="2" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D75" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="2" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D76" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>12</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="2" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>8</v>
@@ -2005,112 +2000,67 @@
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="2" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D78" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" s="2">
-        <v>16</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="D79" s="10">
+        <v>4</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D80" s="2">
         <v>1</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>12</v>
+      <c r="E80" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D81" s="2">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D82" s="2">
-        <v>4</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D83" s="2">
-        <v>1</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D84" s="2">
         <v>16</v>
       </c>
-      <c r="E84" s="6" t="s">
-        <v>105</v>
+      <c r="E81" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Register Top-Level Module and Added Comments
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="129">
   <si>
     <t>Direction</t>
   </si>
@@ -132,15 +132,6 @@
   </si>
   <si>
     <t>rst</t>
-  </si>
-  <si>
-    <t>i2si_sck</t>
-  </si>
-  <si>
-    <t>i2si_ws</t>
-  </si>
-  <si>
-    <t>i2si_sd</t>
   </si>
   <si>
     <t>i2so_sck</t>
@@ -858,8 +849,8 @@
   </sheetPr>
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +907,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -931,7 +922,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -946,7 +937,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -955,13 +946,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -976,7 +967,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -991,7 +982,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -1006,7 +997,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -1021,7 +1012,7 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
@@ -1036,7 +1027,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
@@ -1050,7 +1041,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>33</v>
@@ -1092,7 +1083,7 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
@@ -1107,7 +1098,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -1122,7 +1113,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
@@ -1137,7 +1128,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
@@ -1152,7 +1143,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -1167,7 +1158,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -1182,7 +1173,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
@@ -1197,7 +1188,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -1212,7 +1203,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -1227,7 +1218,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
@@ -1242,7 +1233,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1251,13 +1242,13 @@
         <v>11</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -1266,12 +1257,12 @@
         <v>8</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>33</v>
@@ -1313,7 +1304,7 @@
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>5</v>
@@ -1328,7 +1319,7 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
@@ -1343,7 +1334,7 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1358,7 +1349,7 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1373,7 +1364,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>8</v>
@@ -1388,7 +1379,7 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
@@ -1403,7 +1394,7 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
@@ -1418,7 +1409,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>5</v>
@@ -1432,7 +1423,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>33</v>
@@ -1453,13 +1444,13 @@
         <v>1</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>5</v>
@@ -1468,13 +1459,13 @@
         <v>1</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>5</v>
@@ -1483,13 +1474,13 @@
         <v>1</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>5</v>
@@ -1498,13 +1489,13 @@
         <v>1</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
@@ -1513,13 +1504,13 @@
         <v>1</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>5</v>
@@ -1528,13 +1519,13 @@
         <v>1</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>5</v>
@@ -1543,13 +1534,13 @@
         <v>32</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>5</v>
@@ -1558,13 +1549,13 @@
         <v>8</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>5</v>
@@ -1573,13 +1564,13 @@
         <v>32</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>5</v>
@@ -1588,13 +1579,13 @@
         <v>1</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>5</v>
@@ -1603,13 +1594,13 @@
         <v>1</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>8</v>
@@ -1618,13 +1609,13 @@
         <v>32</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>8</v>
@@ -1633,13 +1624,13 @@
         <v>1</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>5</v>
@@ -1648,13 +1639,13 @@
         <v>1</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>8</v>
@@ -1663,13 +1654,13 @@
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>8</v>
@@ -1678,13 +1669,13 @@
         <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>8</v>
@@ -1693,12 +1684,12 @@
         <v>1</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>33</v>
@@ -1725,7 +1716,7 @@
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>5</v>
@@ -1740,7 +1731,7 @@
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>5</v>
@@ -1755,7 +1746,7 @@
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>5</v>
@@ -1764,13 +1755,13 @@
         <v>1</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>5</v>
@@ -1785,7 +1776,7 @@
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>5</v>
@@ -1794,13 +1785,13 @@
         <v>32</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>8</v>
@@ -1815,7 +1806,7 @@
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>8</v>
@@ -1830,7 +1821,7 @@
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>8</v>
@@ -1845,7 +1836,7 @@
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>8</v>
@@ -1860,7 +1851,7 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>5</v>
@@ -1869,13 +1860,13 @@
         <v>1</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>8</v>
@@ -1884,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1916,7 +1907,7 @@
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>5</v>
@@ -1931,7 +1922,7 @@
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>5</v>
@@ -1940,13 +1931,13 @@
         <v>32</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>5</v>
@@ -1955,28 +1946,28 @@
         <v>1</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>8</v>
@@ -1985,13 +1976,13 @@
         <v>32</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>8</v>
@@ -2000,13 +1991,13 @@
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>5</v>
@@ -2015,13 +2006,13 @@
         <v>1</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>5</v>
@@ -2030,13 +2021,13 @@
         <v>4</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>5</v>
@@ -2045,13 +2036,13 @@
         <v>1</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>5</v>
@@ -2060,7 +2051,7 @@
         <v>16</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Register Interfaces to chip.v
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="139">
   <si>
     <t>Direction</t>
   </si>
@@ -92,9 +92,6 @@
     <t>digital audio serial data</t>
   </si>
   <si>
-    <t>will turn into sticky bit</t>
-  </si>
-  <si>
     <t>read to receive</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>i2so_sd</t>
   </si>
   <si>
-    <t>i2s_inoverrun</t>
-  </si>
-  <si>
     <t>Master Clock</t>
   </si>
   <si>
@@ -236,30 +230,12 @@
     <t>i2c_sda</t>
   </si>
   <si>
-    <t>reg</t>
-  </si>
-  <si>
-    <t>reg_op</t>
-  </si>
-  <si>
-    <t>reg_addr</t>
-  </si>
-  <si>
-    <t>reg_wdata</t>
-  </si>
-  <si>
     <t>reg_rts</t>
   </si>
   <si>
     <t>reg_rtr</t>
   </si>
   <si>
-    <t>reg_rdata</t>
-  </si>
-  <si>
-    <t>reg_xfc</t>
-  </si>
-  <si>
     <t>i2si</t>
   </si>
   <si>
@@ -317,9 +293,6 @@
     <t>rf_mux_en</t>
   </si>
   <si>
-    <t>Select BIST of deserializer</t>
-  </si>
-  <si>
     <t>i2si_data</t>
   </si>
   <si>
@@ -411,13 +384,70 @@
   </si>
   <si>
     <t>ready to receive (for output FIFO)</t>
+  </si>
+  <si>
+    <t>i2c_xfc_write</t>
+  </si>
+  <si>
+    <t>write data transfer complete</t>
+  </si>
+  <si>
+    <t>ro_fifo_overrun</t>
+  </si>
+  <si>
+    <t>i2c_xfc_read</t>
+  </si>
+  <si>
+    <t>rf_i2si_bist_en</t>
+  </si>
+  <si>
+    <t>Select BIST or deserializer</t>
+  </si>
+  <si>
+    <t>0 - no clipping, 1- performs clipping</t>
+  </si>
+  <si>
+    <t>rf_i2si_bist_start_val</t>
+  </si>
+  <si>
+    <t>BIST Start Value</t>
+  </si>
+  <si>
+    <t>chip_reg</t>
+  </si>
+  <si>
+    <t>rf_i2si_bist_incr</t>
+  </si>
+  <si>
+    <t>BIST signal increment value</t>
+  </si>
+  <si>
+    <t>rf_i2si_bist_upper_limit</t>
+  </si>
+  <si>
+    <t>BIST Upper Limit Value</t>
+  </si>
+  <si>
+    <t>trig_fifo_overrun</t>
+  </si>
+  <si>
+    <t>signal to reset I2S input FIFO overrun</t>
+  </si>
+  <si>
+    <t>signal to reset I2S output FIFO underrun</t>
+  </si>
+  <si>
+    <t>needs to be added</t>
+  </si>
+  <si>
+    <t>enable bit for deserializer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,8 +492,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -500,6 +537,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -531,7 +574,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -559,6 +602,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -847,16 +899,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.42578125" bestFit="1" customWidth="1"/>
@@ -882,7 +934,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -892,7 +944,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -901,13 +953,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -922,7 +974,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -931,28 +983,28 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -961,13 +1013,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -976,13 +1028,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -991,13 +1043,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -1006,13 +1058,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
@@ -1021,13 +1073,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
@@ -1036,15 +1088,15 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1053,7 +1105,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
@@ -1068,7 +1120,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -1083,7 +1135,7 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
@@ -1092,13 +1144,13 @@
         <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -1113,7 +1165,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
@@ -1128,7 +1180,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
@@ -1143,7 +1195,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -1158,7 +1210,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -1173,7 +1225,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
@@ -1188,7 +1240,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -1203,7 +1255,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -1218,7 +1270,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
@@ -1233,7 +1285,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1242,13 +1294,13 @@
         <v>11</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -1257,15 +1309,15 @@
         <v>8</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1274,7 +1326,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
@@ -1289,7 +1341,7 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
@@ -1304,52 +1356,52 @@
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="1">
-        <v>1</v>
+      <c r="D31" s="11">
+        <v>12</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="1">
-        <v>32</v>
+      <c r="D32" s="11">
+        <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="1">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1358,279 +1410,281 @@
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D36" s="1">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="1">
-        <v>1</v>
+      <c r="D37" s="11">
+        <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="2">
-        <v>1</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>40</v>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="11">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>41</v>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="2">
-        <v>1</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>42</v>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="1">
+        <v>32</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="2">
-        <v>1</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>43</v>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="1">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="2">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>44</v>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="1">
+        <v>32</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>95</v>
+      <c r="A45" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="2">
+      <c r="A46" s="13"/>
+      <c r="B46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="1">
         <v>32</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>52</v>
+      <c r="E46" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="2">
-        <v>8</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>54</v>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="2">
-        <v>32</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D52" s="2">
         <v>1</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>5</v>
@@ -1639,419 +1693,599 @@
         <v>1</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="2">
+        <v>32</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="2">
+        <v>8</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="2">
+        <v>32</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="2">
+        <v>32</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="9"/>
+      <c r="B68" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="1">
+        <v>1</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="1">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="1">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="1">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="2">
-        <v>1</v>
-      </c>
-      <c r="E55" s="2" t="s">
+      <c r="C75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="1">
+        <v>32</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
-      <c r="B56" s="2" t="s">
+      <c r="C76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="1">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="1">
+        <v>1</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B57" s="1" t="s">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="1">
-        <v>1</v>
-      </c>
-      <c r="E58" s="1" t="s">
+      <c r="C83" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="1">
-        <v>1</v>
-      </c>
-      <c r="E59" s="1" t="s">
+      <c r="C84" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="1">
-        <v>1</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="C85" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="2">
+        <v>32</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="B86" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="2">
+        <v>1</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="B87" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="1">
-        <v>1</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="1">
+      <c r="C87" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="B88" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="2">
         <v>32</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" s="1">
-        <v>1</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" s="1">
-        <v>1</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="1">
-        <v>1</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="1">
-        <v>1</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="1">
-        <v>1</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="1">
-        <v>1</v>
-      </c>
-      <c r="E69" s="1" t="s">
+      <c r="E88" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" s="2">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="2" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="B89" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="2">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="2" t="s">
+      <c r="C89" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" s="2">
-        <v>32</v>
-      </c>
-      <c r="E73" s="2" t="s">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" s="2">
-        <v>1</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="2" t="s">
+      <c r="C90" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="2">
-        <v>32</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="2">
-        <v>1</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D78" s="2">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="2" t="s">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="10">
+        <v>1</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D79" s="10">
-        <v>4</v>
-      </c>
-      <c r="E79" s="6" t="s">
+      <c r="C93" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="2">
+        <v>16</v>
+      </c>
+      <c r="E93" s="6" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" s="2">
-        <v>1</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D81" s="2">
-        <v>16</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed I2S Interface Naming
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="141">
   <si>
     <t>Direction</t>
   </si>
@@ -98,9 +98,6 @@
     <t>serial clock</t>
   </si>
   <si>
-    <t>filter</t>
-  </si>
-  <si>
     <t>chip</t>
   </si>
   <si>
@@ -278,9 +275,6 @@
     <t>rf_i2si_en</t>
   </si>
   <si>
-    <t>inp_sck</t>
-  </si>
-  <si>
     <t>inp_ws</t>
   </si>
   <si>
@@ -305,27 +299,15 @@
     <t>Signal to reset FIFO Overrun</t>
   </si>
   <si>
-    <t>sync_sck</t>
-  </si>
-  <si>
     <t>Synchronized Serial Clock</t>
   </si>
   <si>
-    <t>sck_transition</t>
-  </si>
-  <si>
     <t>Serial Clock Transition</t>
   </si>
   <si>
-    <t>sync_sck_transition</t>
-  </si>
-  <si>
     <t>rst_n</t>
   </si>
   <si>
-    <t>sck_inp</t>
-  </si>
-  <si>
     <t>Serial Clock Level to Pulse Converter</t>
   </si>
   <si>
@@ -441,6 +423,30 @@
   </si>
   <si>
     <t>enable bit for deserializer</t>
+  </si>
+  <si>
+    <t>i2si_sck</t>
+  </si>
+  <si>
+    <t>i2si_ws</t>
+  </si>
+  <si>
+    <t>i2si_sd</t>
+  </si>
+  <si>
+    <t>i2si_sync_sck</t>
+  </si>
+  <si>
+    <t>i2si_sync_sck_transition</t>
+  </si>
+  <si>
+    <t>i2so_sync_sck</t>
+  </si>
+  <si>
+    <t>i2so_sck_transition</t>
+  </si>
+  <si>
+    <t>filt</t>
   </si>
 </sst>
 </file>
@@ -901,8 +907,8 @@
   </sheetPr>
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,7 +940,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -944,7 +950,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -953,13 +959,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -974,7 +980,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -983,28 +989,28 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -1013,13 +1019,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1028,13 +1034,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -1043,13 +1049,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -1058,13 +1064,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
@@ -1073,13 +1079,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
@@ -1088,15 +1094,15 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1105,7 +1111,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
@@ -1120,7 +1126,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -1135,7 +1141,7 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
@@ -1150,7 +1156,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -1165,7 +1171,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
@@ -1180,7 +1186,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
@@ -1195,7 +1201,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -1210,7 +1216,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -1225,7 +1231,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
@@ -1240,7 +1246,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -1255,7 +1261,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -1270,7 +1276,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
@@ -1285,7 +1291,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1294,13 +1300,13 @@
         <v>11</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -1309,15 +1315,15 @@
         <v>8</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1326,7 +1332,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
@@ -1341,7 +1347,7 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
@@ -1356,7 +1362,7 @@
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>5</v>
@@ -1371,7 +1377,7 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
@@ -1386,7 +1392,7 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1395,13 +1401,13 @@
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1416,7 +1422,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1425,13 +1431,13 @@
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
@@ -1440,13 +1446,13 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
@@ -1461,7 +1467,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
@@ -1476,7 +1482,7 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -1485,28 +1491,28 @@
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="11">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="11">
-        <v>1</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>8</v>
@@ -1515,13 +1521,13 @@
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>8</v>
@@ -1530,13 +1536,13 @@
         <v>32</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>8</v>
@@ -1545,13 +1551,13 @@
         <v>8</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>8</v>
@@ -1560,15 +1566,15 @@
         <v>32</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
@@ -1577,13 +1583,13 @@
         <v>1</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>8</v>
@@ -1592,13 +1598,13 @@
         <v>32</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>8</v>
@@ -1607,13 +1613,13 @@
         <v>1</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>8</v>
@@ -1622,13 +1628,13 @@
         <v>1</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>5</v>
@@ -1643,7 +1649,7 @@
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>8</v>
@@ -1657,10 +1663,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -1669,7 +1675,7 @@
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>5</v>
@@ -1678,13 +1684,13 @@
         <v>1</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>5</v>
@@ -1693,13 +1699,13 @@
         <v>1</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>5</v>
@@ -1708,13 +1714,13 @@
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>5</v>
@@ -1723,13 +1729,13 @@
         <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>5</v>
@@ -1738,13 +1744,13 @@
         <v>1</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>5</v>
@@ -1753,13 +1759,13 @@
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>5</v>
@@ -1768,28 +1774,28 @@
         <v>32</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="2">
+        <v>8</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="2">
-        <v>8</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>5</v>
@@ -1798,13 +1804,13 @@
         <v>32</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>5</v>
@@ -1813,28 +1819,28 @@
         <v>1</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>8</v>
@@ -1843,28 +1849,28 @@
         <v>32</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" s="2">
-        <v>1</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>5</v>
@@ -1873,28 +1879,28 @@
         <v>1</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>8</v>
@@ -1903,13 +1909,13 @@
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9"/>
       <c r="B68" s="2" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>8</v>
@@ -1918,15 +1924,15 @@
         <v>1</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -1935,7 +1941,7 @@
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>5</v>
@@ -1950,7 +1956,7 @@
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>5</v>
@@ -1965,7 +1971,7 @@
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>5</v>
@@ -1980,7 +1986,7 @@
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>5</v>
@@ -1989,13 +1995,13 @@
         <v>1</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>5</v>
@@ -2010,7 +2016,7 @@
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>5</v>
@@ -2019,13 +2025,13 @@
         <v>32</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>8</v>
@@ -2040,7 +2046,7 @@
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>8</v>
@@ -2055,7 +2061,7 @@
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>8</v>
@@ -2070,7 +2076,7 @@
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>8</v>
@@ -2085,7 +2091,7 @@
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>5</v>
@@ -2094,13 +2100,13 @@
         <v>1</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>8</v>
@@ -2109,15 +2115,15 @@
         <v>1</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>24</v>
+        <v>140</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
@@ -2126,7 +2132,7 @@
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>5</v>
@@ -2141,7 +2147,7 @@
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>5</v>
@@ -2156,7 +2162,7 @@
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>5</v>
@@ -2165,13 +2171,13 @@
         <v>32</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>5</v>
@@ -2180,13 +2186,13 @@
         <v>1</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>8</v>
@@ -2195,13 +2201,13 @@
         <v>1</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>8</v>
@@ -2210,13 +2216,13 @@
         <v>32</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>8</v>
@@ -2225,13 +2231,13 @@
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>5</v>
@@ -2240,43 +2246,43 @@
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="10">
+        <v>1</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="10">
-        <v>1</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1</v>
+      </c>
+      <c r="E92" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D92" s="2">
-        <v>1</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>5</v>
@@ -2285,7 +2291,7 @@
         <v>16</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added I2C Interface to chip.v
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -907,8 +907,8 @@
   </sheetPr>
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Interface Signal Spreadsheet
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="134">
   <si>
     <t>Direction</t>
   </si>
@@ -44,12 +44,6 @@
     <t>in</t>
   </si>
   <si>
-    <t>I2C Serial Clock</t>
-  </si>
-  <si>
-    <t>I2C Serial Data</t>
-  </si>
-  <si>
     <t>out</t>
   </si>
   <si>
@@ -65,18 +59,12 @@
     <t>ready to send</t>
   </si>
   <si>
-    <t>ready to receive</t>
-  </si>
-  <si>
     <t>read return data</t>
   </si>
   <si>
     <t>read data transfer complete</t>
   </si>
   <si>
-    <t>external pin combines in and out using open drain</t>
-  </si>
-  <si>
     <t>clock</t>
   </si>
   <si>
@@ -104,9 +92,6 @@
     <t>master clock, up to 100MHz</t>
   </si>
   <si>
-    <t>in/out</t>
-  </si>
-  <si>
     <t>I2C serial clock</t>
   </si>
   <si>
@@ -206,33 +191,15 @@
     <t>i2c_wdata</t>
   </si>
   <si>
-    <t>i2c_rts</t>
-  </si>
-  <si>
-    <t>i2c_rtr</t>
-  </si>
-  <si>
     <t>i2c_rdata</t>
   </si>
   <si>
-    <t>i2c_xfc</t>
-  </si>
-  <si>
     <t>I2C serial data</t>
   </si>
   <si>
     <t>i2c_scl</t>
   </si>
   <si>
-    <t>i2c_sda</t>
-  </si>
-  <si>
-    <t>reg_rts</t>
-  </si>
-  <si>
-    <t>reg_rtr</t>
-  </si>
-  <si>
     <t>i2si</t>
   </si>
   <si>
@@ -254,18 +221,6 @@
     <t>1- performs clipping 0- no cliping</t>
   </si>
   <si>
-    <t>rf_i2c_reg_indir_addr</t>
-  </si>
-  <si>
-    <t>ro_i2c_reg_indir_data</t>
-  </si>
-  <si>
-    <t>address register used for indirect addressing via i2c</t>
-  </si>
-  <si>
-    <t>data access register</t>
-  </si>
-  <si>
     <t>rf_filter_coeff#</t>
   </si>
   <si>
@@ -275,12 +230,6 @@
     <t>rf_i2si_en</t>
   </si>
   <si>
-    <t>inp_ws</t>
-  </si>
-  <si>
-    <t>inp_sd</t>
-  </si>
-  <si>
     <t>Enable bit for deserializer</t>
   </si>
   <si>
@@ -419,9 +368,6 @@
     <t>signal to reset I2S output FIFO underrun</t>
   </si>
   <si>
-    <t>needs to be added</t>
-  </si>
-  <si>
     <t>enable bit for deserializer</t>
   </si>
   <si>
@@ -447,13 +393,46 @@
   </si>
   <si>
     <t>filt</t>
+  </si>
+  <si>
+    <t>i2c_addr_bits</t>
+  </si>
+  <si>
+    <t>i2c_waddr</t>
+  </si>
+  <si>
+    <t>3 LSB I2C address select</t>
+  </si>
+  <si>
+    <t>1- write, 0- read</t>
+  </si>
+  <si>
+    <t>reset not</t>
+  </si>
+  <si>
+    <t>write data address</t>
+  </si>
+  <si>
+    <t>write data</t>
+  </si>
+  <si>
+    <t>trig_filter_ovf_flag_clear</t>
+  </si>
+  <si>
+    <t>signal to reset filter overflow flag</t>
+  </si>
+  <si>
+    <t>ro_filter_ovf_flag</t>
+  </si>
+  <si>
+    <t>Filter Overflow Flag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,11 +473,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,7 +480,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -528,18 +502,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,7 +542,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -598,25 +560,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -905,10 +858,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,7 +893,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -950,7 +903,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -959,13 +912,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -974,13 +927,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -989,28 +942,28 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -1019,311 +972,311 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>17</v>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>6</v>
+      <c r="D16" s="2">
+        <v>3</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>7</v>
+      <c r="D17" s="2">
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D21" s="2">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2">
         <v>8</v>
       </c>
-      <c r="D22" s="2">
-        <v>1</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="7" t="s">
-        <v>76</v>
+      <c r="B26" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="2">
-        <v>11</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>78</v>
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="8" t="s">
-        <v>77</v>
+      <c r="B27" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="2">
-        <v>8</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>79</v>
+        <v>1</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1332,7 +1285,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
@@ -1341,13 +1294,13 @@
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
@@ -1356,43 +1309,43 @@
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="11">
-        <v>12</v>
+      <c r="D31" s="9">
+        <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="9">
         <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1401,13 +1354,13 @@
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1416,13 +1369,13 @@
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1431,13 +1384,13 @@
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
@@ -1446,227 +1399,225 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="11">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>14</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="9">
         <v>8</v>
       </c>
-      <c r="D38" s="1">
-        <v>1</v>
-      </c>
       <c r="E38" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="11">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1">
         <v>1</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D41" s="9">
+        <v>3</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D42" s="1">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D43" s="1">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="1">
         <v>8</v>
       </c>
-      <c r="D44" s="1">
+      <c r="E44" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="1">
         <v>32</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
+      <c r="A46" s="8"/>
       <c r="B46" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="1">
         <v>32</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
       <c r="E47" s="1" t="s">
-        <v>129</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -1675,22 +1626,22 @@
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>5</v>
@@ -1699,13 +1650,13 @@
         <v>1</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>5</v>
@@ -1714,13 +1665,13 @@
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>5</v>
@@ -1729,13 +1680,13 @@
         <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>5</v>
@@ -1744,13 +1695,13 @@
         <v>1</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>5</v>
@@ -1759,13 +1710,13 @@
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>5</v>
@@ -1774,13 +1725,13 @@
         <v>32</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>5</v>
@@ -1789,13 +1740,13 @@
         <v>8</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>5</v>
@@ -1804,13 +1755,13 @@
         <v>32</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>5</v>
@@ -1819,13 +1770,13 @@
         <v>1</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>5</v>
@@ -1834,43 +1785,43 @@
         <v>1</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D63" s="2">
         <v>32</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D64" s="2">
         <v>1</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>5</v>
@@ -1879,60 +1830,60 @@
         <v>1</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D66" s="2">
         <v>1</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="9"/>
+      <c r="A68" s="7"/>
       <c r="B68" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -1941,7 +1892,7 @@
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>5</v>
@@ -1950,13 +1901,13 @@
         <v>1</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>5</v>
@@ -1965,13 +1916,13 @@
         <v>1</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>5</v>
@@ -1980,13 +1931,13 @@
         <v>1</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>5</v>
@@ -1995,13 +1946,13 @@
         <v>1</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>5</v>
@@ -2010,13 +1961,13 @@
         <v>1</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>5</v>
@@ -2025,73 +1976,73 @@
         <v>32</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D76" s="1">
         <v>1</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D77" s="1">
         <v>1</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D78" s="1">
         <v>1</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D79" s="1">
         <v>1</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>5</v>
@@ -2100,30 +2051,30 @@
         <v>1</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D81" s="1">
         <v>1</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
@@ -2132,7 +2083,7 @@
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>5</v>
@@ -2141,13 +2092,13 @@
         <v>1</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="2" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>5</v>
@@ -2156,13 +2107,13 @@
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="2" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>5</v>
@@ -2171,13 +2122,13 @@
         <v>32</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="2" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>5</v>
@@ -2186,58 +2137,58 @@
         <v>1</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="2" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D87" s="2">
         <v>1</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="2" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D88" s="2">
         <v>32</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="2" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D89" s="2">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="2" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>5</v>
@@ -2246,52 +2197,82 @@
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="2" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D91" s="10">
-        <v>1</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>73</v>
+      <c r="D91" s="2">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="2" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D92" s="2">
         <v>1</v>
       </c>
-      <c r="E92" s="6" t="s">
-        <v>75</v>
+      <c r="E92" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93" s="10">
+        <v>3</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="B94" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="2">
+        <v>1</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="B95" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95" s="2">
         <v>16</v>
       </c>
-      <c r="E93" s="6" t="s">
-        <v>81</v>
+      <c r="E95" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Source Code Folder
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="140">
   <si>
     <t>Direction</t>
   </si>
@@ -432,6 +432,18 @@
   </si>
   <si>
     <t>filt_out_data</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>JA</t>
+  </si>
+  <si>
+    <t>I2S</t>
+  </si>
+  <si>
+    <t>JB</t>
   </si>
 </sst>
 </file>
@@ -518,7 +530,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -541,6 +553,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -548,7 +569,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -576,6 +597,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -864,10 +888,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +904,7 @@
     <col min="6" max="6" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -897,7 +921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -906,7 +930,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>27</v>
@@ -921,7 +945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>76</v>
@@ -935,8 +959,14 @@
       <c r="E4" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>113</v>
@@ -950,8 +980,14 @@
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>114</v>
@@ -966,7 +1002,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>115</v>
@@ -981,7 +1017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>29</v>
@@ -996,7 +1032,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>30</v>
@@ -1011,7 +1047,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>31</v>
@@ -1026,7 +1062,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>120</v>
@@ -1041,7 +1077,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>57</v>
@@ -1056,7 +1092,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>50</v>
@@ -1071,7 +1107,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>51</v>
@@ -1086,7 +1122,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
@@ -1097,7 +1133,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
FPGA Work and Updated Verilog Code
</commit_message>
<xml_diff>
--- a/proj_asic/docs/rtl_description.xlsx
+++ b/proj_asic/docs/rtl_description.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="162">
   <si>
     <t>Direction</t>
   </si>
@@ -437,9 +437,6 @@
     <t>FPGA Port</t>
   </si>
   <si>
-    <t>JB1</t>
-  </si>
-  <si>
     <t>JB2</t>
   </si>
   <si>
@@ -459,6 +456,60 @@
   </si>
   <si>
     <t>JA3</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>V11</t>
+  </si>
+  <si>
+    <t>V15</t>
+  </si>
+  <si>
+    <t>JB7</t>
+  </si>
+  <si>
+    <t>K16</t>
+  </si>
+  <si>
+    <t>JB8</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>JB9</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>JB10</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>D18,C17,G13</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>F14</t>
+  </si>
+  <si>
+    <t>D17</t>
+  </si>
+  <si>
+    <t>crystal</t>
   </si>
 </sst>
 </file>
@@ -583,7 +634,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -613,14 +664,18 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -945,8 +1000,8 @@
   </sheetPr>
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,6 +1012,7 @@
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -975,8 +1031,11 @@
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>136</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -987,6 +1046,8 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1002,6 +1063,12 @@
       <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="F3" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -1017,8 +1084,13 @@
       <c r="E4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="F4" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1034,11 +1106,13 @@
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
+      <c r="F5" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1054,11 +1128,13 @@
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="F6" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -1074,8 +1150,11 @@
       <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>139</v>
+      <c r="F7" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1092,8 +1171,11 @@
       <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>140</v>
+      <c r="F8" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1110,7 +1192,12 @@
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -1126,7 +1213,12 @@
       <c r="E10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -1142,8 +1234,11 @@
       <c r="E11" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>141</v>
+      <c r="F11" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1160,8 +1255,11 @@
       <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>142</v>
+      <c r="F12" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1178,8 +1276,11 @@
       <c r="E13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>143</v>
+      <c r="F13" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1196,8 +1297,11 @@
       <c r="E14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>144</v>
+      <c r="F14" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>